<commit_message>
updated compilation file citation DOIs
</commit_message>
<xml_diff>
--- a/data/vgp_database/Absaroka_volcanics.xlsx
+++ b/data/vgp_database/Absaroka_volcanics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimingzhang/Github/Gallo_etal_2023_APWP_construction/data/vgp_database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267B8A27-220D-9642-BAC0-936AA4338BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6832C8-929E-D545-A3F5-F245208B6B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8320" yWindow="500" windowWidth="33600" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29580" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2205" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2069" uniqueCount="198">
   <si>
     <t>Name:</t>
   </si>
@@ -626,418 +626,10 @@
     <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</t>
   </si>
   <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.026</t>
+    <t>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</t>
   </si>
   <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.027</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.028</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.029</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.030</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.031</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.032</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.033</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.034</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.035</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.036</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.037</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.038</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.039</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.040</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.041</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.042</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.043</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.044</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.045</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.046</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.047</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.048</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.049</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.050</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.051</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.052</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.053</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.054</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.055</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.056</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.057</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.058</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.059</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.060</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.061</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.062</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.063</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.064</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.065</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.066</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.067</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.068</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.069</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.070</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.071</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.072</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.073</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.074</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.075</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.076</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.077</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.078</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.079</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.080</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.081</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.082</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.083</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.084</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.085</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.086</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.087</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.088</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.089</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.090</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.091</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.092</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.093</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.094</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.095</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.096</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.097</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.098</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.099</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.100</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.101</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.102</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.103</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.104</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.105</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.106</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.107</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.108</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.109</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.110</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.111</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.112</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.113</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.114</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.115</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.116</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.117</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.118</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.119</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.120</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.121</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.122</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.123</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.124</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.125</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.126</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.127</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.128</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.129</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.130</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.131</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.132</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.133</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.134</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.135</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.136</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.137</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.138</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.139</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.140</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.141</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.142</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.143</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.144</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.145</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.146</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.147</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.148</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.149</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.150</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.151</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.152</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.153</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.154</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.155</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.156</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.157</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.158</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.159</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.160</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.161</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.162</t>
-  </si>
-  <si>
-    <t>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.163</t>
+    <t>10.1016/j.tecto.2009.12.025</t>
   </si>
 </sst>
 </file>
@@ -1511,8 +1103,8 @@
   </sheetPr>
   <dimension ref="A1:AQ1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AP12" sqref="AP12:AP150"/>
+    <sheetView tabSelected="1" topLeftCell="AI106" workbookViewId="0">
+      <selection activeCell="AP113" sqref="AP113:AP150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1549,6 +1141,7 @@
     <col min="32" max="32" width="11.83203125" customWidth="1"/>
     <col min="33" max="34" width="12.6640625" customWidth="1"/>
     <col min="35" max="35" width="14" customWidth="1"/>
+    <col min="38" max="38" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2598,8 +2191,9 @@
       <c r="AO13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP13" s="40" t="s">
-        <v>196</v>
+      <c r="AP13" s="40" t="str">
+        <f>AP12</f>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="14" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2706,8 +2300,9 @@
       <c r="AO14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP14" s="40" t="s">
-        <v>197</v>
+      <c r="AP14" s="40" t="str">
+        <f t="shared" ref="AP14:AP55" si="0">AP13</f>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="15" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2816,8 +2411,9 @@
       <c r="AO15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP15" s="40" t="s">
-        <v>198</v>
+      <c r="AP15" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="16" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2928,8 +2524,9 @@
       <c r="AO16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP16" s="40" t="s">
-        <v>199</v>
+      <c r="AP16" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="17" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3038,8 +2635,9 @@
       <c r="AO17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP17" s="40" t="s">
-        <v>200</v>
+      <c r="AP17" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="18" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3150,8 +2748,9 @@
       <c r="AO18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP18" s="40" t="s">
-        <v>201</v>
+      <c r="AP18" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="19" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3262,8 +2861,9 @@
       <c r="AO19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP19" s="40" t="s">
-        <v>202</v>
+      <c r="AP19" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="20" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3372,8 +2972,9 @@
       <c r="AO20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP20" s="40" t="s">
-        <v>203</v>
+      <c r="AP20" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="21" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3480,8 +3081,9 @@
       <c r="AO21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP21" s="40" t="s">
-        <v>204</v>
+      <c r="AP21" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="22" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3588,8 +3190,9 @@
       <c r="AO22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP22" s="40" t="s">
-        <v>205</v>
+      <c r="AP22" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="23" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3698,8 +3301,9 @@
       <c r="AO23" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP23" s="40" t="s">
-        <v>206</v>
+      <c r="AP23" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="24" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3806,8 +3410,9 @@
       <c r="AO24" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP24" s="40" t="s">
-        <v>207</v>
+      <c r="AP24" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="25" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3916,8 +3521,9 @@
       <c r="AO25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP25" s="40" t="s">
-        <v>208</v>
+      <c r="AP25" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="26" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4026,8 +3632,9 @@
       <c r="AO26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP26" s="40" t="s">
-        <v>209</v>
+      <c r="AP26" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="27" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4134,8 +3741,9 @@
       <c r="AO27" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP27" s="40" t="s">
-        <v>210</v>
+      <c r="AP27" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="28" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4244,8 +3852,9 @@
       <c r="AO28" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP28" s="40" t="s">
-        <v>211</v>
+      <c r="AP28" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="29" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4352,8 +3961,9 @@
       <c r="AO29" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP29" s="40" t="s">
-        <v>212</v>
+      <c r="AP29" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="30" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4460,8 +4070,9 @@
       <c r="AO30" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP30" s="40" t="s">
-        <v>213</v>
+      <c r="AP30" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="31" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4568,8 +4179,9 @@
       <c r="AO31" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP31" s="40" t="s">
-        <v>214</v>
+      <c r="AP31" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="32" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4678,8 +4290,9 @@
       <c r="AO32" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP32" s="40" t="s">
-        <v>215</v>
+      <c r="AP32" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="33" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4786,8 +4399,9 @@
       <c r="AO33" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP33" s="40" t="s">
-        <v>216</v>
+      <c r="AP33" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="34" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4894,8 +4508,9 @@
       <c r="AO34" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP34" s="40" t="s">
-        <v>217</v>
+      <c r="AP34" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="35" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5000,8 +4615,9 @@
       <c r="AO35" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP35" s="40" t="s">
-        <v>218</v>
+      <c r="AP35" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="36" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5108,8 +4724,9 @@
       <c r="AO36" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP36" s="40" t="s">
-        <v>219</v>
+      <c r="AP36" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="37" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5218,8 +4835,9 @@
       <c r="AO37" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP37" s="40" t="s">
-        <v>220</v>
+      <c r="AP37" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="38" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5328,8 +4946,9 @@
       <c r="AO38" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP38" s="40" t="s">
-        <v>221</v>
+      <c r="AP38" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="39" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5436,8 +5055,9 @@
       <c r="AO39" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP39" s="40" t="s">
-        <v>222</v>
+      <c r="AP39" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="40" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5546,8 +5166,9 @@
       <c r="AO40" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP40" s="40" t="s">
-        <v>223</v>
+      <c r="AP40" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="41" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5656,8 +5277,9 @@
       <c r="AO41" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP41" s="40" t="s">
-        <v>224</v>
+      <c r="AP41" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="42" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5764,8 +5386,9 @@
       <c r="AO42" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP42" s="40" t="s">
-        <v>225</v>
+      <c r="AP42" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="43" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5872,8 +5495,9 @@
       <c r="AO43" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP43" s="40" t="s">
-        <v>226</v>
+      <c r="AP43" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="44" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5982,8 +5606,9 @@
       <c r="AO44" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP44" s="40" t="s">
-        <v>227</v>
+      <c r="AP44" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="45" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6092,8 +5717,9 @@
       <c r="AO45" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP45" s="40" t="s">
-        <v>228</v>
+      <c r="AP45" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="46" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6202,8 +5828,9 @@
       <c r="AO46" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP46" s="40" t="s">
-        <v>229</v>
+      <c r="AP46" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="47" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6310,8 +5937,9 @@
       <c r="AO47" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP47" s="40" t="s">
-        <v>230</v>
+      <c r="AP47" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="48" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6416,8 +6044,9 @@
       <c r="AO48" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP48" s="40" t="s">
-        <v>231</v>
+      <c r="AP48" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="49" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6526,8 +6155,9 @@
       <c r="AO49" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP49" s="40" t="s">
-        <v>232</v>
+      <c r="AP49" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="50" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6636,8 +6266,9 @@
       <c r="AO50" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP50" s="40" t="s">
-        <v>233</v>
+      <c r="AP50" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="51" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6742,8 +6373,9 @@
       <c r="AO51" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP51" s="40" t="s">
-        <v>234</v>
+      <c r="AP51" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="52" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6852,8 +6484,9 @@
       <c r="AO52" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP52" s="40" t="s">
-        <v>235</v>
+      <c r="AP52" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="53" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6962,8 +6595,9 @@
       <c r="AO53" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP53" s="40" t="s">
-        <v>236</v>
+      <c r="AP53" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="54" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7070,8 +6704,9 @@
       <c r="AO54" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP54" s="40" t="s">
-        <v>237</v>
+      <c r="AP54" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="55" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7180,8 +6815,9 @@
       <c r="AO55" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP55" s="40" t="s">
-        <v>238</v>
+      <c r="AP55" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1029/JB082i020p03039:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="56" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7291,7 +6927,7 @@
         <v>53</v>
       </c>
       <c r="AP56" s="40" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7400,8 +7036,9 @@
       <c r="AO57" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP57" s="40" t="s">
-        <v>240</v>
+      <c r="AP57" s="40" t="str">
+        <f>AP56</f>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="58" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7510,8 +7147,9 @@
       <c r="AO58" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP58" s="40" t="s">
-        <v>241</v>
+      <c r="AP58" s="40" t="str">
+        <f t="shared" ref="AP58:AP111" si="1">AP57</f>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="59" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7620,8 +7258,9 @@
       <c r="AO59" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP59" s="40" t="s">
-        <v>242</v>
+      <c r="AP59" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="60" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7730,8 +7369,9 @@
       <c r="AO60" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP60" s="40" t="s">
-        <v>243</v>
+      <c r="AP60" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="61" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7840,8 +7480,9 @@
       <c r="AO61" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP61" s="40" t="s">
-        <v>244</v>
+      <c r="AP61" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="62" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7950,8 +7591,9 @@
       <c r="AO62" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP62" s="40" t="s">
-        <v>245</v>
+      <c r="AP62" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="63" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8060,8 +7702,9 @@
       <c r="AO63" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP63" s="40" t="s">
-        <v>246</v>
+      <c r="AP63" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="64" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8170,8 +7813,9 @@
       <c r="AO64" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP64" s="40" t="s">
-        <v>247</v>
+      <c r="AP64" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="65" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8280,8 +7924,9 @@
       <c r="AO65" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP65" s="40" t="s">
-        <v>248</v>
+      <c r="AP65" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="66" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8390,8 +8035,9 @@
       <c r="AO66" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP66" s="40" t="s">
-        <v>249</v>
+      <c r="AP66" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="67" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8500,8 +8146,9 @@
       <c r="AO67" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP67" s="40" t="s">
-        <v>250</v>
+      <c r="AP67" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="68" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8610,8 +8257,9 @@
       <c r="AO68" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP68" s="40" t="s">
-        <v>251</v>
+      <c r="AP68" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="69" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8720,8 +8368,9 @@
       <c r="AO69" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP69" s="40" t="s">
-        <v>252</v>
+      <c r="AP69" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="70" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8830,8 +8479,9 @@
       <c r="AO70" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP70" s="40" t="s">
-        <v>253</v>
+      <c r="AP70" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="71" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8940,8 +8590,9 @@
       <c r="AO71" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP71" s="40" t="s">
-        <v>254</v>
+      <c r="AP71" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="72" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9050,8 +8701,9 @@
       <c r="AO72" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP72" s="40" t="s">
-        <v>255</v>
+      <c r="AP72" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="73" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9160,8 +8812,9 @@
       <c r="AO73" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP73" s="40" t="s">
-        <v>256</v>
+      <c r="AP73" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="74" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9270,8 +8923,9 @@
       <c r="AO74" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP74" s="40" t="s">
-        <v>257</v>
+      <c r="AP74" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="75" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9380,8 +9034,9 @@
       <c r="AO75" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP75" s="40" t="s">
-        <v>258</v>
+      <c r="AP75" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="76" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9478,8 +9133,9 @@
       <c r="AO76" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP76" s="40" t="s">
-        <v>259</v>
+      <c r="AP76" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="77" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9588,8 +9244,9 @@
       <c r="AO77" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP77" s="40" t="s">
-        <v>260</v>
+      <c r="AP77" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="78" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9698,8 +9355,9 @@
       <c r="AO78" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP78" s="40" t="s">
-        <v>261</v>
+      <c r="AP78" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="79" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9808,8 +9466,9 @@
       <c r="AO79" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP79" s="40" t="s">
-        <v>262</v>
+      <c r="AP79" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="80" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9918,8 +9577,9 @@
       <c r="AO80" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP80" s="40" t="s">
-        <v>263</v>
+      <c r="AP80" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="81" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10028,8 +9688,9 @@
       <c r="AO81" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP81" s="40" t="s">
-        <v>264</v>
+      <c r="AP81" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="82" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10138,8 +9799,9 @@
       <c r="AO82" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP82" s="40" t="s">
-        <v>265</v>
+      <c r="AP82" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="83" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10248,8 +9910,9 @@
       <c r="AO83" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP83" s="40" t="s">
-        <v>266</v>
+      <c r="AP83" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="84" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10358,8 +10021,9 @@
       <c r="AO84" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP84" s="40" t="s">
-        <v>267</v>
+      <c r="AP84" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="85" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10468,8 +10132,9 @@
       <c r="AO85" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP85" s="40" t="s">
-        <v>268</v>
+      <c r="AP85" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="86" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10578,8 +10243,9 @@
       <c r="AO86" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP86" s="40" t="s">
-        <v>269</v>
+      <c r="AP86" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="87" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10688,8 +10354,9 @@
       <c r="AO87" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP87" s="40" t="s">
-        <v>270</v>
+      <c r="AP87" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="88" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10798,8 +10465,9 @@
       <c r="AO88" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP88" s="40" t="s">
-        <v>271</v>
+      <c r="AP88" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="89" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10908,8 +10576,9 @@
       <c r="AO89" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP89" s="40" t="s">
-        <v>272</v>
+      <c r="AP89" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="90" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11018,8 +10687,9 @@
       <c r="AO90" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP90" s="40" t="s">
-        <v>273</v>
+      <c r="AP90" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="91" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11128,8 +10798,9 @@
       <c r="AO91" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP91" s="40" t="s">
-        <v>274</v>
+      <c r="AP91" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="92" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11238,8 +10909,9 @@
       <c r="AO92" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP92" s="40" t="s">
-        <v>275</v>
+      <c r="AP92" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="93" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11348,8 +11020,9 @@
       <c r="AO93" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP93" s="40" t="s">
-        <v>276</v>
+      <c r="AP93" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="94" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11458,8 +11131,9 @@
       <c r="AO94" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP94" s="40" t="s">
-        <v>277</v>
+      <c r="AP94" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="95" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11568,8 +11242,9 @@
       <c r="AO95" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP95" s="40" t="s">
-        <v>278</v>
+      <c r="AP95" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="96" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11678,8 +11353,9 @@
       <c r="AO96" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP96" s="40" t="s">
-        <v>279</v>
+      <c r="AP96" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="97" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11788,8 +11464,9 @@
       <c r="AO97" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP97" s="40" t="s">
-        <v>280</v>
+      <c r="AP97" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="98" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11898,8 +11575,9 @@
       <c r="AO98" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP98" s="40" t="s">
-        <v>281</v>
+      <c r="AP98" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="99" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12008,8 +11686,9 @@
       <c r="AO99" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP99" s="40" t="s">
-        <v>282</v>
+      <c r="AP99" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="100" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12118,8 +11797,9 @@
       <c r="AO100" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP100" s="40" t="s">
-        <v>283</v>
+      <c r="AP100" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="101" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12228,8 +11908,9 @@
       <c r="AO101" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP101" s="40" t="s">
-        <v>284</v>
+      <c r="AP101" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="102" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12338,8 +12019,9 @@
       <c r="AO102" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP102" s="40" t="s">
-        <v>285</v>
+      <c r="AP102" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="103" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12448,8 +12130,9 @@
       <c r="AO103" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP103" s="40" t="s">
-        <v>286</v>
+      <c r="AP103" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="104" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12546,8 +12229,9 @@
       <c r="AO104" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP104" s="40" t="s">
-        <v>287</v>
+      <c r="AP104" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="105" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12656,8 +12340,9 @@
       <c r="AO105" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP105" s="40" t="s">
-        <v>288</v>
+      <c r="AP105" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="106" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12766,8 +12451,9 @@
       <c r="AO106" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP106" s="40" t="s">
-        <v>289</v>
+      <c r="AP106" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="107" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12876,8 +12562,9 @@
       <c r="AO107" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP107" s="40" t="s">
-        <v>290</v>
+      <c r="AP107" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="108" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12986,8 +12673,9 @@
       <c r="AO108" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP108" s="40" t="s">
-        <v>291</v>
+      <c r="AP108" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="109" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -13096,8 +12784,9 @@
       <c r="AO109" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP109" s="40" t="s">
-        <v>292</v>
+      <c r="AP109" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="110" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -13206,8 +12895,9 @@
       <c r="AO110" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP110" s="40" t="s">
-        <v>293</v>
+      <c r="AP110" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="111" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -13304,8 +12994,9 @@
       <c r="AO111" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AP111" s="40" t="s">
-        <v>294</v>
+      <c r="AP111" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>10.1016/0012-821X(87)90128-2:10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="112" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -13413,7 +13104,7 @@
         <v>58</v>
       </c>
       <c r="AP112" s="40" t="s">
-        <v>295</v>
+        <v>197</v>
       </c>
     </row>
     <row r="113" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -13520,8 +13211,9 @@
       <c r="AO113" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP113" s="40" t="s">
-        <v>296</v>
+      <c r="AP113" s="40" t="str">
+        <f>AP112</f>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="114" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -13624,8 +13316,9 @@
       <c r="AO114" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP114" s="40" t="s">
-        <v>297</v>
+      <c r="AP114" s="40" t="str">
+        <f t="shared" ref="AP114:AP150" si="2">AP113</f>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="115" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -13730,8 +13423,9 @@
       <c r="AO115" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP115" s="40" t="s">
-        <v>298</v>
+      <c r="AP115" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="116" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -13834,8 +13528,9 @@
       <c r="AO116" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP116" s="40" t="s">
-        <v>299</v>
+      <c r="AP116" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="117" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -13938,8 +13633,9 @@
       <c r="AO117" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP117" s="40" t="s">
-        <v>300</v>
+      <c r="AP117" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="118" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14042,8 +13738,9 @@
       <c r="AO118" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP118" s="40" t="s">
-        <v>301</v>
+      <c r="AP118" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="119" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14146,8 +13843,9 @@
       <c r="AO119" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP119" s="40" t="s">
-        <v>302</v>
+      <c r="AP119" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="120" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14250,8 +13948,9 @@
       <c r="AO120" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP120" s="40" t="s">
-        <v>303</v>
+      <c r="AP120" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="121" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14354,8 +14053,9 @@
       <c r="AO121" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP121" s="40" t="s">
-        <v>304</v>
+      <c r="AP121" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="122" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14458,8 +14158,9 @@
       <c r="AO122" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP122" s="40" t="s">
-        <v>305</v>
+      <c r="AP122" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="123" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14566,8 +14267,9 @@
       <c r="AO123" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP123" s="40" t="s">
-        <v>306</v>
+      <c r="AP123" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="124" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14670,8 +14372,9 @@
       <c r="AO124" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP124" s="40" t="s">
-        <v>307</v>
+      <c r="AP124" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="125" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14774,8 +14477,9 @@
       <c r="AO125" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP125" s="40" t="s">
-        <v>308</v>
+      <c r="AP125" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="126" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14876,8 +14580,9 @@
       <c r="AO126" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP126" s="40" t="s">
-        <v>309</v>
+      <c r="AP126" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="127" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14980,8 +14685,9 @@
       <c r="AO127" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP127" s="40" t="s">
-        <v>310</v>
+      <c r="AP127" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="128" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15084,8 +14790,9 @@
       <c r="AO128" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP128" s="40" t="s">
-        <v>311</v>
+      <c r="AP128" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="129" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15192,8 +14899,9 @@
       <c r="AO129" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP129" s="40" t="s">
-        <v>312</v>
+      <c r="AP129" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="130" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15300,8 +15008,9 @@
       <c r="AO130" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP130" s="40" t="s">
-        <v>313</v>
+      <c r="AP130" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="131" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15404,8 +15113,9 @@
       <c r="AO131" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP131" s="40" t="s">
-        <v>314</v>
+      <c r="AP131" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="132" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15508,8 +15218,9 @@
       <c r="AO132" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP132" s="40" t="s">
-        <v>315</v>
+      <c r="AP132" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="133" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15612,8 +15323,9 @@
       <c r="AO133" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP133" s="40" t="s">
-        <v>316</v>
+      <c r="AP133" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="134" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15716,8 +15428,9 @@
       <c r="AO134" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP134" s="40" t="s">
-        <v>317</v>
+      <c r="AP134" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="135" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15824,8 +15537,9 @@
       <c r="AO135" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP135" s="40" t="s">
-        <v>318</v>
+      <c r="AP135" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="136" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -15932,8 +15646,9 @@
       <c r="AO136" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP136" s="40" t="s">
-        <v>319</v>
+      <c r="AP136" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="137" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16034,8 +15749,9 @@
       <c r="AO137" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP137" s="40" t="s">
-        <v>320</v>
+      <c r="AP137" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="138" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16138,8 +15854,9 @@
       <c r="AO138" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP138" s="40" t="s">
-        <v>321</v>
+      <c r="AP138" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="139" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16240,8 +15957,9 @@
       <c r="AO139" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP139" s="40" t="s">
-        <v>322</v>
+      <c r="AP139" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="140" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16348,8 +16066,9 @@
       <c r="AO140" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP140" s="40" t="s">
-        <v>323</v>
+      <c r="AP140" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="141" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16452,8 +16171,9 @@
       <c r="AO141" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP141" s="40" t="s">
-        <v>324</v>
+      <c r="AP141" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="142" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16560,8 +16280,9 @@
       <c r="AO142" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP142" s="40" t="s">
-        <v>325</v>
+      <c r="AP142" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="143" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16668,8 +16389,9 @@
       <c r="AO143" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP143" s="40" t="s">
-        <v>326</v>
+      <c r="AP143" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="144" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16776,8 +16498,9 @@
       <c r="AO144" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP144" s="40" t="s">
-        <v>327</v>
+      <c r="AP144" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="145" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16884,8 +16607,9 @@
       <c r="AO145" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP145" s="40" t="s">
-        <v>328</v>
+      <c r="AP145" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="146" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16992,8 +16716,9 @@
       <c r="AO146" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP146" s="40" t="s">
-        <v>329</v>
+      <c r="AP146" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="147" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17100,8 +16825,9 @@
       <c r="AO147" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP147" s="40" t="s">
-        <v>330</v>
+      <c r="AP147" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="148" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17204,8 +16930,9 @@
       <c r="AO148" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP148" s="40" t="s">
-        <v>331</v>
+      <c r="AP148" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="149" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17308,8 +17035,9 @@
       <c r="AO149" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP149" s="40" t="s">
-        <v>332</v>
+      <c r="AP149" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="150" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17412,8 +17140,9 @@
       <c r="AO150" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AP150" s="40" t="s">
-        <v>333</v>
+      <c r="AP150" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>10.1016/j.tecto.2009.12.025</v>
       </c>
     </row>
     <row r="151" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -27070,7 +26799,8 @@
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="AP12" r:id="rId1" display="https://doi.org/10.1029/JB082i020p03039" xr:uid="{7D7BF64A-D0CB-F44F-BD3B-B9FC01317329}"/>
-    <hyperlink ref="AP13:AP150" r:id="rId2" display="https://doi.org/10.1029/JB082i020p03039" xr:uid="{D570F568-662A-D547-A39F-973B170A1C04}"/>
+    <hyperlink ref="AP13" r:id="rId2" display="https://doi.org/10.1029/JB082i020p03039" xr:uid="{AFF64D90-BA53-7B42-9113-8EF6B2D7A0D0}"/>
+    <hyperlink ref="AP14:AP55" r:id="rId3" display="https://doi.org/10.1029/JB082i020p03039" xr:uid="{E366BB05-F6B9-9449-9D34-6C421803DF64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>